<commit_message>
added some test code
</commit_message>
<xml_diff>
--- a/Lab7-FinalProjectHardware/Deliverables/Port_Assignments.xlsx
+++ b/Lab7-FinalProjectHardware/Deliverables/Port_Assignments.xlsx
@@ -499,17 +499,16 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>